<commit_message>
Add new metadata report for Akurana
</commit_message>
<xml_diff>
--- a/Akurana_Metadata_Report.xlsx
+++ b/Akurana_Metadata_Report.xlsx
@@ -605,21 +605,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NOV</t>
+          <t>JAN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30/11-01/11</t>
+          <t>10/01-01/01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>11/01, 12/01, 13/01, 14/01, 15/01, 16/01, 17/01, 18/01, 19/01, 20/01, 21/01, 22/01, 23/01, 24/01, 25/01, 26/01, 27/01, 28/01, 29/01, 30/01, 31/01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">

</xml_diff>

<commit_message>
Add/update metadata report for Akurana
</commit_message>
<xml_diff>
--- a/Akurana_Metadata_Report.xlsx
+++ b/Akurana_Metadata_Report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -783,6 +783,211 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>JAN</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10/01-01/01</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>11/01, 12/01, 13/01, 14/01, 15/01, 16/01, 17/01, 18/01, 19/01, 20/01, 21/01, 22/01, 23/01, 24/01, 25/01, 26/01, 27/01, 28/01, 29/01, 30/01, 31/01</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Akurana</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update metadata report for Akurana
</commit_message>
<xml_diff>
--- a/Akurana_Metadata_Report.xlsx
+++ b/Akurana_Metadata_Report.xlsx
@@ -605,21 +605,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DEC</t>
+          <t>JAN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>31/12-01/12</t>
+          <t>10/01-01/01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>11/01, 12/01, 13/01, 14/01, 15/01, 16/01, 17/01, 18/01, 19/01, 20/01, 21/01, 22/01, 23/01, 24/01, 25/01, 26/01, 27/01, 28/01, 29/01, 30/01, 31/01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">

</xml_diff>